<commit_message>
initial work on preprocessing and "error reporting" (print and abort atm)
</commit_message>
<xml_diff>
--- a/Prebuild Milestone.xlsx
+++ b/Prebuild Milestone.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Cog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9FC892F-A9D0-4C61-8D4D-BC6C2D5391BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEC4C565-3D1A-49CC-A85B-47D4F9E7D93C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="45972" yWindow="2892" windowWidth="30936" windowHeight="16896" xr2:uid="{262B2709-DD1D-48CB-ABA6-E417142083D9}"/>
   </bookViews>
@@ -295,10 +295,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -641,7 +641,7 @@
   <dimension ref="B2:P38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="H7" sqref="H7:I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -667,27 +667,27 @@
       <c r="C4" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="17"/>
-      <c r="E4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="17"/>
       <c r="F4" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="18"/>
+      <c r="G4" s="17"/>
       <c r="H4" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="18"/>
+      <c r="I4" s="17"/>
       <c r="J4" s="4" t="s">
         <v>11</v>
       </c>
       <c r="K4" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="L4" s="17"/>
-      <c r="M4" s="17"/>
-      <c r="N4" s="17"/>
-      <c r="O4" s="17"/>
-      <c r="P4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
+      <c r="N4" s="18"/>
+      <c r="O4" s="18"/>
+      <c r="P4" s="17"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B5" s="4">
@@ -703,12 +703,12 @@
       </c>
       <c r="G5" s="15"/>
       <c r="H5" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I5" s="15"/>
       <c r="J5" s="10">
         <f>IF(F5, 1-H5/F5,"")</f>
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="K5" s="13"/>
       <c r="L5" s="14"/>
@@ -731,12 +731,12 @@
       </c>
       <c r="G6" s="15"/>
       <c r="H6" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I6" s="15"/>
       <c r="J6" s="10">
         <f>IF(F6, 1-H6/F6,"")</f>
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="K6" s="13" t="s">
         <v>34</v>
@@ -1170,15 +1170,15 @@
         <f>SUM(F5:F24)</f>
         <v>15</v>
       </c>
-      <c r="G25" s="18"/>
+      <c r="G25" s="17"/>
       <c r="H25" s="16">
         <f>SUM(H5:H24)</f>
-        <v>9</v>
-      </c>
-      <c r="I25" s="18"/>
+        <v>7</v>
+      </c>
+      <c r="I25" s="17"/>
       <c r="J25" s="7">
         <f>1-H25/F25</f>
-        <v>0.4</v>
+        <v>0.53333333333333333</v>
       </c>
       <c r="K25" s="13"/>
       <c r="L25" s="14"/>
@@ -1210,7 +1210,7 @@
       </c>
       <c r="C27" s="8">
         <f ca="1">NOW()</f>
-        <v>43775.766626157405</v>
+        <v>43778.828929745374</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3" t="s">
@@ -1218,7 +1218,7 @@
       </c>
       <c r="F27" s="3">
         <f ca="1">_xlfn.DAYS(C27,C28)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G27" s="3"/>
       <c r="H27" s="3" t="s">
@@ -1226,7 +1226,7 @@
       </c>
       <c r="I27" s="3">
         <f ca="1">I28+I29</f>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="J27" s="3" t="s">
         <v>16</v>
@@ -1256,7 +1256,7 @@
       </c>
       <c r="F28" s="6">
         <f ca="1">MIN(C31, MAX(0, NETWORKDAYS(C28,C27)-1))</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G28" s="3"/>
       <c r="H28" s="3" t="s">
@@ -1264,7 +1264,7 @@
       </c>
       <c r="I28" s="3">
         <f ca="1">F28*L28</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J28" s="3" t="s">
         <v>16</v>
@@ -1293,7 +1293,7 @@
       </c>
       <c r="F29" s="6">
         <f ca="1">F27-F28</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G29" s="3"/>
       <c r="H29" t="s">
@@ -1301,7 +1301,7 @@
       </c>
       <c r="I29">
         <f ca="1">F29*L29</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J29" s="3" t="s">
         <v>16</v>
@@ -1359,7 +1359,7 @@
       </c>
       <c r="F32">
         <f ca="1">I27</f>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="G32" t="s">
         <v>16</v>
@@ -1384,7 +1384,7 @@
       </c>
       <c r="F33" s="1">
         <f ca="1">MAX(0, F25-I27)</f>
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>16</v>
@@ -1396,7 +1396,7 @@
       </c>
       <c r="F34">
         <f>H25</f>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G34" t="s">
         <v>16</v>
@@ -1418,7 +1418,7 @@
       </c>
       <c r="F35" s="1">
         <f ca="1">F34-F33</f>
-        <v>-4</v>
+        <v>-1</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>16</v>
@@ -1450,82 +1450,6 @@
     </row>
   </sheetData>
   <mergeCells count="88">
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="K24:P24"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="K25:P25"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="K16:P16"/>
-    <mergeCell ref="K17:P17"/>
-    <mergeCell ref="K18:P18"/>
-    <mergeCell ref="K19:P19"/>
-    <mergeCell ref="K20:P20"/>
-    <mergeCell ref="K21:P21"/>
-    <mergeCell ref="K22:P22"/>
-    <mergeCell ref="K23:P23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="K4:P4"/>
-    <mergeCell ref="K5:P5"/>
-    <mergeCell ref="K6:P6"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="K7:P7"/>
-    <mergeCell ref="K8:P8"/>
-    <mergeCell ref="K9:P9"/>
-    <mergeCell ref="K10:P10"/>
     <mergeCell ref="K11:P11"/>
     <mergeCell ref="K12:P12"/>
     <mergeCell ref="H16:I16"/>
@@ -1538,6 +1462,82 @@
     <mergeCell ref="K13:P13"/>
     <mergeCell ref="K14:P14"/>
     <mergeCell ref="K15:P15"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="K4:P4"/>
+    <mergeCell ref="K5:P5"/>
+    <mergeCell ref="K6:P6"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="K7:P7"/>
+    <mergeCell ref="K8:P8"/>
+    <mergeCell ref="K9:P9"/>
+    <mergeCell ref="K10:P10"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="K16:P16"/>
+    <mergeCell ref="K17:P17"/>
+    <mergeCell ref="K18:P18"/>
+    <mergeCell ref="K19:P19"/>
+    <mergeCell ref="K20:P20"/>
+    <mergeCell ref="K24:P24"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="K25:P25"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="K21:P21"/>
+    <mergeCell ref="K22:P22"/>
+    <mergeCell ref="K23:P23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F19:G19"/>
   </mergeCells>
   <conditionalFormatting sqref="F35">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">

</xml_diff>

<commit_message>
header parser looking for COGTYPE(), GENERATED_BODY; and inclusion of *.generated.h
</commit_message>
<xml_diff>
--- a/Prebuild Milestone.xlsx
+++ b/Prebuild Milestone.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Cog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEC4C565-3D1A-49CC-A85B-47D4F9E7D93C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A8D8B4-7DA4-45F5-AD68-24B0B4FEB1A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="45972" yWindow="2892" windowWidth="30936" windowHeight="16896" xr2:uid="{262B2709-DD1D-48CB-ABA6-E417142083D9}"/>
   </bookViews>
@@ -641,7 +641,7 @@
   <dimension ref="B2:P38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7:I7"/>
+      <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -791,12 +791,12 @@
       </c>
       <c r="G8" s="15"/>
       <c r="H8" s="13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I8" s="15"/>
       <c r="J8" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="K8" s="13" t="s">
         <v>38</v>
@@ -1173,12 +1173,12 @@
       <c r="G25" s="17"/>
       <c r="H25" s="16">
         <f>SUM(H5:H24)</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I25" s="17"/>
       <c r="J25" s="7">
         <f>1-H25/F25</f>
-        <v>0.53333333333333333</v>
+        <v>0.6</v>
       </c>
       <c r="K25" s="13"/>
       <c r="L25" s="14"/>
@@ -1210,7 +1210,7 @@
       </c>
       <c r="C27" s="8">
         <f ca="1">NOW()</f>
-        <v>43778.828929745374</v>
+        <v>43779.101650810182</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3" t="s">
@@ -1218,7 +1218,7 @@
       </c>
       <c r="F27" s="3">
         <f ca="1">_xlfn.DAYS(C27,C28)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G27" s="3"/>
       <c r="H27" s="3" t="s">
@@ -1226,7 +1226,7 @@
       </c>
       <c r="I27" s="3">
         <f ca="1">I28+I29</f>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="J27" s="3" t="s">
         <v>16</v>
@@ -1293,7 +1293,7 @@
       </c>
       <c r="F29" s="6">
         <f ca="1">F27-F28</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G29" s="3"/>
       <c r="H29" t="s">
@@ -1301,7 +1301,7 @@
       </c>
       <c r="I29">
         <f ca="1">F29*L29</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J29" s="3" t="s">
         <v>16</v>
@@ -1359,7 +1359,7 @@
       </c>
       <c r="F32">
         <f ca="1">I27</f>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G32" t="s">
         <v>16</v>
@@ -1384,7 +1384,7 @@
       </c>
       <c r="F33" s="1">
         <f ca="1">MAX(0, F25-I27)</f>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>16</v>
@@ -1396,7 +1396,7 @@
       </c>
       <c r="F34">
         <f>H25</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G34" t="s">
         <v>16</v>
@@ -1418,7 +1418,7 @@
       </c>
       <c r="F35" s="1">
         <f ca="1">F34-F33</f>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
header files with cogypes now generates generated header and source files, some slight planning for future milestones
</commit_message>
<xml_diff>
--- a/Prebuild Milestone.xlsx
+++ b/Prebuild Milestone.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Cog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A8D8B4-7DA4-45F5-AD68-24B0B4FEB1A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFE38DA0-F4DE-4423-AE5C-70520B12D779}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="45972" yWindow="2892" windowWidth="30936" windowHeight="16896" xr2:uid="{262B2709-DD1D-48CB-ABA6-E417142083D9}"/>
   </bookViews>
@@ -286,10 +286,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -641,7 +641,7 @@
   <dimension ref="B2:P38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H46" sqref="H46"/>
+      <selection activeCell="H8" sqref="H8:I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -696,26 +696,26 @@
       <c r="C5" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="14"/>
-      <c r="E5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="14"/>
       <c r="F5" s="13">
         <v>4</v>
       </c>
-      <c r="G5" s="15"/>
+      <c r="G5" s="14"/>
       <c r="H5" s="13">
         <v>0</v>
       </c>
-      <c r="I5" s="15"/>
+      <c r="I5" s="14"/>
       <c r="J5" s="10">
         <f>IF(F5, 1-H5/F5,"")</f>
         <v>1</v>
       </c>
       <c r="K5" s="13"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="14"/>
-      <c r="O5" s="14"/>
-      <c r="P5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="14"/>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B6" s="4">
@@ -724,16 +724,16 @@
       <c r="C6" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="D6" s="14"/>
-      <c r="E6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="14"/>
       <c r="F6" s="13">
         <v>4</v>
       </c>
-      <c r="G6" s="15"/>
+      <c r="G6" s="14"/>
       <c r="H6" s="13">
         <v>0</v>
       </c>
-      <c r="I6" s="15"/>
+      <c r="I6" s="14"/>
       <c r="J6" s="10">
         <f>IF(F6, 1-H6/F6,"")</f>
         <v>1</v>
@@ -741,11 +741,11 @@
       <c r="K6" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="14"/>
-      <c r="P6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="14"/>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B7" s="4">
@@ -754,16 +754,16 @@
       <c r="C7" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="14"/>
       <c r="F7" s="13">
         <v>3</v>
       </c>
-      <c r="G7" s="15"/>
+      <c r="G7" s="14"/>
       <c r="H7" s="13">
         <v>3</v>
       </c>
-      <c r="I7" s="15"/>
+      <c r="I7" s="14"/>
       <c r="J7" s="10">
         <f t="shared" ref="J7:J24" si="0">IF(F7, 1-H7/F7,"")</f>
         <v>0</v>
@@ -771,11 +771,11 @@
       <c r="K7" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="14"/>
-      <c r="O7" s="14"/>
-      <c r="P7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="15"/>
+      <c r="P7" s="14"/>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B8" s="4">
@@ -784,388 +784,388 @@
       <c r="C8" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="14"/>
       <c r="F8" s="13">
         <v>4</v>
       </c>
-      <c r="G8" s="15"/>
+      <c r="G8" s="14"/>
       <c r="H8" s="13">
-        <v>3</v>
-      </c>
-      <c r="I8" s="15"/>
+        <v>0</v>
+      </c>
+      <c r="I8" s="14"/>
       <c r="J8" s="10">
         <f t="shared" si="0"/>
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="K8" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
-      <c r="O8" s="14"/>
-      <c r="P8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="14"/>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B9" s="4">
         <v>5</v>
       </c>
       <c r="C9" s="13"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="14"/>
       <c r="F9" s="13"/>
-      <c r="G9" s="15"/>
+      <c r="G9" s="14"/>
       <c r="H9" s="13"/>
-      <c r="I9" s="15"/>
+      <c r="I9" s="14"/>
       <c r="J9" s="10" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K9" s="13"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="14"/>
-      <c r="O9" s="14"/>
-      <c r="P9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="14"/>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B10" s="4">
         <v>6</v>
       </c>
       <c r="C10" s="13"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="14"/>
       <c r="F10" s="13"/>
-      <c r="G10" s="15"/>
+      <c r="G10" s="14"/>
       <c r="H10" s="13"/>
-      <c r="I10" s="15"/>
+      <c r="I10" s="14"/>
       <c r="J10" s="10" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K10" s="13"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="14"/>
-      <c r="O10" s="14"/>
-      <c r="P10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="15"/>
+      <c r="O10" s="15"/>
+      <c r="P10" s="14"/>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B11" s="4">
         <v>7</v>
       </c>
       <c r="C11" s="13"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="14"/>
       <c r="F11" s="13"/>
-      <c r="G11" s="15"/>
+      <c r="G11" s="14"/>
       <c r="H11" s="13"/>
-      <c r="I11" s="15"/>
+      <c r="I11" s="14"/>
       <c r="J11" s="10" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K11" s="13"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="14"/>
-      <c r="O11" s="14"/>
-      <c r="P11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="14"/>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B12" s="5">
         <v>8</v>
       </c>
       <c r="C12" s="13"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="14"/>
       <c r="F12" s="13"/>
-      <c r="G12" s="15"/>
+      <c r="G12" s="14"/>
       <c r="H12" s="13"/>
-      <c r="I12" s="15"/>
+      <c r="I12" s="14"/>
       <c r="J12" s="10" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K12" s="13"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="14"/>
-      <c r="O12" s="14"/>
-      <c r="P12" s="15"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="15"/>
+      <c r="P12" s="14"/>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B13" s="5">
         <v>9</v>
       </c>
       <c r="C13" s="13"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="14"/>
       <c r="F13" s="13"/>
-      <c r="G13" s="15"/>
+      <c r="G13" s="14"/>
       <c r="H13" s="13"/>
-      <c r="I13" s="15"/>
+      <c r="I13" s="14"/>
       <c r="J13" s="10" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K13" s="13"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="14"/>
-      <c r="O13" s="14"/>
-      <c r="P13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="15"/>
+      <c r="P13" s="14"/>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B14" s="5">
         <v>10</v>
       </c>
       <c r="C14" s="13"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="14"/>
       <c r="F14" s="13"/>
-      <c r="G14" s="15"/>
+      <c r="G14" s="14"/>
       <c r="H14" s="13"/>
-      <c r="I14" s="15"/>
+      <c r="I14" s="14"/>
       <c r="J14" s="10" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K14" s="13"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="14"/>
-      <c r="O14" s="14"/>
-      <c r="P14" s="15"/>
+      <c r="L14" s="15"/>
+      <c r="M14" s="15"/>
+      <c r="N14" s="15"/>
+      <c r="O14" s="15"/>
+      <c r="P14" s="14"/>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B15" s="5">
         <v>11</v>
       </c>
       <c r="C15" s="13"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="14"/>
       <c r="F15" s="13"/>
-      <c r="G15" s="15"/>
+      <c r="G15" s="14"/>
       <c r="H15" s="13"/>
-      <c r="I15" s="15"/>
+      <c r="I15" s="14"/>
       <c r="J15" s="10" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K15" s="13"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="14"/>
-      <c r="O15" s="14"/>
-      <c r="P15" s="15"/>
+      <c r="L15" s="15"/>
+      <c r="M15" s="15"/>
+      <c r="N15" s="15"/>
+      <c r="O15" s="15"/>
+      <c r="P15" s="14"/>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B16" s="5">
         <v>12</v>
       </c>
       <c r="C16" s="13"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="14"/>
       <c r="F16" s="13"/>
-      <c r="G16" s="15"/>
+      <c r="G16" s="14"/>
       <c r="H16" s="13"/>
-      <c r="I16" s="15"/>
+      <c r="I16" s="14"/>
       <c r="J16" s="10" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K16" s="13"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="14"/>
-      <c r="O16" s="14"/>
-      <c r="P16" s="15"/>
+      <c r="L16" s="15"/>
+      <c r="M16" s="15"/>
+      <c r="N16" s="15"/>
+      <c r="O16" s="15"/>
+      <c r="P16" s="14"/>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B17" s="5">
         <v>13</v>
       </c>
       <c r="C17" s="13"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="14"/>
       <c r="F17" s="13"/>
-      <c r="G17" s="15"/>
+      <c r="G17" s="14"/>
       <c r="H17" s="13"/>
-      <c r="I17" s="15"/>
+      <c r="I17" s="14"/>
       <c r="J17" s="10" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K17" s="13"/>
-      <c r="L17" s="14"/>
-      <c r="M17" s="14"/>
-      <c r="N17" s="14"/>
-      <c r="O17" s="14"/>
-      <c r="P17" s="15"/>
+      <c r="L17" s="15"/>
+      <c r="M17" s="15"/>
+      <c r="N17" s="15"/>
+      <c r="O17" s="15"/>
+      <c r="P17" s="14"/>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B18" s="5">
         <v>14</v>
       </c>
       <c r="C18" s="13"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="14"/>
       <c r="F18" s="13"/>
-      <c r="G18" s="15"/>
+      <c r="G18" s="14"/>
       <c r="H18" s="13"/>
-      <c r="I18" s="15"/>
+      <c r="I18" s="14"/>
       <c r="J18" s="10" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K18" s="13"/>
-      <c r="L18" s="14"/>
-      <c r="M18" s="14"/>
-      <c r="N18" s="14"/>
-      <c r="O18" s="14"/>
-      <c r="P18" s="15"/>
+      <c r="L18" s="15"/>
+      <c r="M18" s="15"/>
+      <c r="N18" s="15"/>
+      <c r="O18" s="15"/>
+      <c r="P18" s="14"/>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B19" s="5">
         <v>15</v>
       </c>
       <c r="C19" s="13"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="14"/>
       <c r="F19" s="13"/>
-      <c r="G19" s="15"/>
+      <c r="G19" s="14"/>
       <c r="H19" s="13"/>
-      <c r="I19" s="15"/>
+      <c r="I19" s="14"/>
       <c r="J19" s="10" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K19" s="13"/>
-      <c r="L19" s="14"/>
-      <c r="M19" s="14"/>
-      <c r="N19" s="14"/>
-      <c r="O19" s="14"/>
-      <c r="P19" s="15"/>
+      <c r="L19" s="15"/>
+      <c r="M19" s="15"/>
+      <c r="N19" s="15"/>
+      <c r="O19" s="15"/>
+      <c r="P19" s="14"/>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B20" s="5">
         <v>16</v>
       </c>
       <c r="C20" s="13"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="14"/>
       <c r="F20" s="13"/>
-      <c r="G20" s="15"/>
+      <c r="G20" s="14"/>
       <c r="H20" s="13"/>
-      <c r="I20" s="15"/>
+      <c r="I20" s="14"/>
       <c r="J20" s="10" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K20" s="13"/>
-      <c r="L20" s="14"/>
-      <c r="M20" s="14"/>
-      <c r="N20" s="14"/>
-      <c r="O20" s="14"/>
-      <c r="P20" s="15"/>
+      <c r="L20" s="15"/>
+      <c r="M20" s="15"/>
+      <c r="N20" s="15"/>
+      <c r="O20" s="15"/>
+      <c r="P20" s="14"/>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B21" s="5">
         <v>17</v>
       </c>
       <c r="C21" s="13"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="14"/>
       <c r="F21" s="13"/>
-      <c r="G21" s="15"/>
+      <c r="G21" s="14"/>
       <c r="H21" s="13"/>
-      <c r="I21" s="15"/>
+      <c r="I21" s="14"/>
       <c r="J21" s="10" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K21" s="13"/>
-      <c r="L21" s="14"/>
-      <c r="M21" s="14"/>
-      <c r="N21" s="14"/>
-      <c r="O21" s="14"/>
-      <c r="P21" s="15"/>
+      <c r="L21" s="15"/>
+      <c r="M21" s="15"/>
+      <c r="N21" s="15"/>
+      <c r="O21" s="15"/>
+      <c r="P21" s="14"/>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B22" s="5">
         <v>18</v>
       </c>
       <c r="C22" s="13"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="14"/>
       <c r="F22" s="13"/>
-      <c r="G22" s="15"/>
+      <c r="G22" s="14"/>
       <c r="H22" s="13"/>
-      <c r="I22" s="15"/>
+      <c r="I22" s="14"/>
       <c r="J22" s="10" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K22" s="13"/>
-      <c r="L22" s="14"/>
-      <c r="M22" s="14"/>
-      <c r="N22" s="14"/>
-      <c r="O22" s="14"/>
-      <c r="P22" s="15"/>
+      <c r="L22" s="15"/>
+      <c r="M22" s="15"/>
+      <c r="N22" s="15"/>
+      <c r="O22" s="15"/>
+      <c r="P22" s="14"/>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B23" s="5">
         <v>19</v>
       </c>
       <c r="C23" s="13"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="14"/>
       <c r="F23" s="13"/>
-      <c r="G23" s="15"/>
+      <c r="G23" s="14"/>
       <c r="H23" s="13"/>
-      <c r="I23" s="15"/>
+      <c r="I23" s="14"/>
       <c r="J23" s="10" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K23" s="13"/>
-      <c r="L23" s="14"/>
-      <c r="M23" s="14"/>
-      <c r="N23" s="14"/>
-      <c r="O23" s="14"/>
-      <c r="P23" s="15"/>
+      <c r="L23" s="15"/>
+      <c r="M23" s="15"/>
+      <c r="N23" s="15"/>
+      <c r="O23" s="15"/>
+      <c r="P23" s="14"/>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B24" s="5">
         <v>20</v>
       </c>
       <c r="C24" s="13"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="14"/>
       <c r="F24" s="13"/>
-      <c r="G24" s="15"/>
+      <c r="G24" s="14"/>
       <c r="H24" s="13"/>
-      <c r="I24" s="15"/>
+      <c r="I24" s="14"/>
       <c r="J24" s="10" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K24" s="13"/>
-      <c r="L24" s="14"/>
-      <c r="M24" s="14"/>
-      <c r="N24" s="14"/>
-      <c r="O24" s="14"/>
-      <c r="P24" s="15"/>
+      <c r="L24" s="15"/>
+      <c r="M24" s="15"/>
+      <c r="N24" s="15"/>
+      <c r="O24" s="15"/>
+      <c r="P24" s="14"/>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B25" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C25" s="13"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="14"/>
       <c r="F25" s="16">
         <f>SUM(F5:F24)</f>
         <v>15</v>
@@ -1173,19 +1173,19 @@
       <c r="G25" s="17"/>
       <c r="H25" s="16">
         <f>SUM(H5:H24)</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I25" s="17"/>
       <c r="J25" s="7">
         <f>1-H25/F25</f>
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="K25" s="13"/>
-      <c r="L25" s="14"/>
-      <c r="M25" s="14"/>
-      <c r="N25" s="14"/>
-      <c r="O25" s="14"/>
-      <c r="P25" s="15"/>
+      <c r="L25" s="15"/>
+      <c r="M25" s="15"/>
+      <c r="N25" s="15"/>
+      <c r="O25" s="15"/>
+      <c r="P25" s="14"/>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B26" s="3"/>
@@ -1210,7 +1210,7 @@
       </c>
       <c r="C27" s="8">
         <f ca="1">NOW()</f>
-        <v>43779.101650810182</v>
+        <v>43782.931876967596</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3" t="s">
@@ -1218,7 +1218,7 @@
       </c>
       <c r="F27" s="3">
         <f ca="1">_xlfn.DAYS(C27,C28)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G27" s="3"/>
       <c r="H27" s="3" t="s">
@@ -1226,7 +1226,7 @@
       </c>
       <c r="I27" s="3">
         <f ca="1">I28+I29</f>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="J27" s="3" t="s">
         <v>16</v>
@@ -1256,7 +1256,7 @@
       </c>
       <c r="F28" s="6">
         <f ca="1">MIN(C31, MAX(0, NETWORKDAYS(C28,C27)-1))</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G28" s="3"/>
       <c r="H28" s="3" t="s">
@@ -1264,7 +1264,7 @@
       </c>
       <c r="I28" s="3">
         <f ca="1">F28*L28</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="J28" s="3" t="s">
         <v>16</v>
@@ -1359,7 +1359,7 @@
       </c>
       <c r="F32">
         <f ca="1">I27</f>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G32" t="s">
         <v>16</v>
@@ -1384,7 +1384,7 @@
       </c>
       <c r="F33" s="1">
         <f ca="1">MAX(0, F25-I27)</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>16</v>
@@ -1396,7 +1396,7 @@
       </c>
       <c r="F34">
         <f>H25</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G34" t="s">
         <v>16</v>
@@ -1463,26 +1463,29 @@
     <mergeCell ref="K14:P14"/>
     <mergeCell ref="K15:P15"/>
     <mergeCell ref="H11:I11"/>
+    <mergeCell ref="K16:P16"/>
+    <mergeCell ref="K17:P17"/>
+    <mergeCell ref="K18:P18"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="K4:P4"/>
+    <mergeCell ref="K5:P5"/>
+    <mergeCell ref="K6:P6"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F8:G8"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="H5:I5"/>
     <mergeCell ref="H6:I6"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="H8:I8"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="K4:P4"/>
-    <mergeCell ref="K5:P5"/>
-    <mergeCell ref="K6:P6"/>
     <mergeCell ref="H10:I10"/>
     <mergeCell ref="K7:P7"/>
     <mergeCell ref="K8:P8"/>
     <mergeCell ref="K9:P9"/>
     <mergeCell ref="K10:P10"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H9:I9"/>
     <mergeCell ref="C24:E24"/>
     <mergeCell ref="C25:E25"/>
     <mergeCell ref="C10:E10"/>
@@ -1501,9 +1504,10 @@
     <mergeCell ref="C8:E8"/>
     <mergeCell ref="C9:E9"/>
     <mergeCell ref="C5:E5"/>
-    <mergeCell ref="K16:P16"/>
-    <mergeCell ref="K17:P17"/>
-    <mergeCell ref="K18:P18"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C19:E19"/>
     <mergeCell ref="K19:P19"/>
     <mergeCell ref="K20:P20"/>
     <mergeCell ref="K24:P24"/>
@@ -1519,25 +1523,21 @@
     <mergeCell ref="H24:I24"/>
     <mergeCell ref="F25:G25"/>
     <mergeCell ref="H25:I25"/>
+    <mergeCell ref="H19:I19"/>
     <mergeCell ref="F15:G15"/>
     <mergeCell ref="F16:G16"/>
     <mergeCell ref="F22:G22"/>
     <mergeCell ref="F24:G24"/>
     <mergeCell ref="F20:G20"/>
     <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F19:G19"/>
     <mergeCell ref="F10:G10"/>
     <mergeCell ref="F11:G11"/>
     <mergeCell ref="F12:G12"/>
     <mergeCell ref="F13:G13"/>
     <mergeCell ref="F14:G14"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F19:G19"/>
   </mergeCells>
   <conditionalFormatting sqref="F35">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">

</xml_diff>